<commit_message>
fix html report overwriting + add regex usage
</commit_message>
<xml_diff>
--- a/Data/test_data.xlsx
+++ b/Data/test_data.xlsx
@@ -57,7 +57,7 @@
     <t>automationAssessment@iLABQuality.com</t>
   </si>
   <si>
-    <t>09 Sep 2020 17:14:42</t>
+    <t>09 Sep 2020 21:50:25</t>
   </si>
   <si>
     <t>Pass</t>
@@ -72,7 +72,7 @@
     <t>Sihle Pangumso</t>
   </si>
   <si>
-    <t>09 Sep 2020 17:16:37</t>
+    <t>09 Sep 2020 21:52:06</t>
   </si>
 </sst>
 </file>
@@ -618,8 +618,8 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId3"/>
-    <hyperlink ref="D3" r:id="rId4"/>
+    <hyperlink ref="D2" r:id="rId13"/>
+    <hyperlink ref="D3" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>

</xml_diff>